<commit_message>
Adding labs 24, 26-29
</commit_message>
<xml_diff>
--- a/24_cardiopulmonary_resuscitation/24_cardiopulmonary_resuscitation_data.xlsx
+++ b/24_cardiopulmonary_resuscitation/24_cardiopulmonary_resuscitation_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>CPR Data</t>
   </si>
@@ -39,18 +39,6 @@
     <t>Blood Pressure(mmHg)</t>
   </si>
   <si>
-    <t>123/78</t>
-  </si>
-  <si>
-    <t>35/18</t>
-  </si>
-  <si>
-    <t>35/19</t>
-  </si>
-  <si>
-    <t>34/19</t>
-  </si>
-  <si>
     <t>Cardiac Output(mL/min)</t>
   </si>
   <si>
@@ -69,18 +57,6 @@
     <t>Blood pH(unitless)(arterial/venous)</t>
   </si>
   <si>
-    <t>7.40/7.36</t>
-  </si>
-  <si>
-    <t>7.43/7.36</t>
-  </si>
-  <si>
-    <t>7.42/7.35</t>
-  </si>
-  <si>
-    <t>7.45/7.32</t>
-  </si>
-  <si>
     <t>Blood [Lac-]</t>
   </si>
   <si>
@@ -88,6 +64,27 @@
   </si>
   <si>
     <t>Symp Activity(Hz)</t>
+  </si>
+  <si>
+    <t>124/79</t>
+  </si>
+  <si>
+    <t>34/24</t>
+  </si>
+  <si>
+    <t>35/26</t>
+  </si>
+  <si>
+    <t>7.43/7.38</t>
+  </si>
+  <si>
+    <t>7.45/7.38</t>
+  </si>
+  <si>
+    <t>7.44/7.38</t>
+  </si>
+  <si>
+    <t>7.48/7.35</t>
   </si>
 </sst>
 </file>
@@ -202,11 +199,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -516,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E14"/>
     </sheetView>
   </sheetViews>
@@ -545,88 +542,88 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75.75" thickBot="1">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="3">
+        <v>5346</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1758</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1777</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B5" s="3">
+        <v>72</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75.75" thickBot="1">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4">
-        <v>5361</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1531</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1544</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4">
-        <v>72</v>
-      </c>
-      <c r="C5" s="4">
-        <v>100</v>
-      </c>
-      <c r="D5" s="4">
-        <v>100</v>
-      </c>
-      <c r="E5" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4">
-        <v>74</v>
-      </c>
-      <c r="C6" s="4">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4">
-        <v>15</v>
+      <c r="B6" s="3">
+        <v>75</v>
+      </c>
+      <c r="C6" s="3">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="44.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C7" s="7">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="D7" s="7">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="E7" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
@@ -638,19 +635,19 @@
     </row>
     <row r="9" spans="1:5" ht="29.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7">
         <v>91</v>
       </c>
       <c r="C9" s="7">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D9" s="7">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E9" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
@@ -661,85 +658,85 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="75.75" thickBot="1">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3</v>
+      <c r="E12" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="4">
-        <v>6.8</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="3">
         <v>2</v>
       </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6</v>
+      <c r="E13" s="3">
+        <v>6.1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
         <v>1.5</v>
       </c>
-      <c r="C14" s="4">
-        <v>2.9</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2.2999999999999998</v>
+      <c r="C14" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Lab 24 Annotations, it also cannot be completed
</commit_message>
<xml_diff>
--- a/24_cardiopulmonary_resuscitation/24_cardiopulmonary_resuscitation_data.xlsx
+++ b/24_cardiopulmonary_resuscitation/24_cardiopulmonary_resuscitation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>CPR Data</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Arterial pO2(mmHg)</t>
   </si>
   <si>
-    <t>Blood pH(unitless)(arterial/venous)</t>
-  </si>
-  <si>
     <t>Blood [Lac-]</t>
   </si>
   <si>
@@ -75,16 +72,19 @@
     <t>35/26</t>
   </si>
   <si>
-    <t>7.43/7.38</t>
-  </si>
-  <si>
-    <t>7.45/7.38</t>
-  </si>
-  <si>
-    <t>7.44/7.38</t>
-  </si>
-  <si>
-    <t>7.48/7.35</t>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>120/79</t>
+  </si>
+  <si>
+    <t>Blood pH(unitless)(venous)</t>
+  </si>
+  <si>
+    <t>In HumMod, attempting to activate CPR causes the entire program to crash. This lab is also not possible to complete as a result.</t>
   </si>
 </sst>
 </file>
@@ -106,12 +106,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -205,6 +211,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -216,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,20 +526,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -540,25 +568,49 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="60.75" thickBot="1">
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="33.75" customHeight="1" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75.75" thickBot="1">
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -574,8 +626,17 @@
       <c r="E4" s="3">
         <v>1598</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45.75" thickBot="1">
+      <c r="G4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5468</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -591,8 +652,17 @@
       <c r="E5" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" thickBot="1">
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3">
+        <v>72</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" customHeight="1" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -608,75 +678,121 @@
       <c r="E6" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="44.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3">
+        <v>76</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="42" customHeight="1" thickBot="1">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>194</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>85</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>84</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8">
+        <v>211</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" hidden="1" thickBot="1">
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>91</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>51</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <v>47</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="75.75" thickBot="1">
-      <c r="A11" s="4" t="s">
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="8">
+        <v>93</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="6.75" customHeight="1" thickBot="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" ht="35.25" customHeight="1" thickBot="1">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.35</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A12" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>1.7</v>
@@ -690,10 +806,19 @@
       <c r="E12" s="3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="45.75" thickBot="1">
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>6.5</v>
@@ -707,10 +832,19 @@
       <c r="E13" s="3">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="45.75" thickBot="1">
+      <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="26.25" customHeight="1" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>1.5</v>
@@ -724,19 +858,53 @@
       <c r="E14" s="3">
         <v>2.2000000000000002</v>
       </c>
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="21">
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>